<commit_message>
updated assignment 1 solution, slides and coding exercise files
</commit_message>
<xml_diff>
--- a/data/codingLiberal.xlsx
+++ b/data/codingLiberal.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Documents\github\HertieTextAnalysis\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.haber\Documents\github\HertieTextAnalysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6348"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="141">
   <si>
     <t>Timestamp</t>
   </si>
@@ -397,12 +397,57 @@
   </si>
   <si>
     <t>607.1 Multiculturalism General: Positive</t>
+  </si>
+  <si>
+    <t>mariaz09@gmail.com</t>
+  </si>
+  <si>
+    <t>408 Economic Goals</t>
+  </si>
+  <si>
+    <t>604 Traditional Morality: Negative</t>
+  </si>
+  <si>
+    <t>412 Controlled Economy: Positive</t>
+  </si>
+  <si>
+    <t>adhikariraju1@gmail.com</t>
+  </si>
+  <si>
+    <t>401 Free-Market Economy: Positive</t>
+  </si>
+  <si>
+    <t>601.1 National Way of Life General: Positive</t>
+  </si>
+  <si>
+    <t>305.6 Rehabilitation and Compensation</t>
+  </si>
+  <si>
+    <t>603 Traditional Morality: Positive</t>
+  </si>
+  <si>
+    <t>507 Education Limitation</t>
+  </si>
+  <si>
+    <t>406 Protectionism: Positive</t>
+  </si>
+  <si>
+    <t>m.monteiro@mpp.hertie-school.org</t>
+  </si>
+  <si>
+    <t>607.3 Indigenous rights: Positive</t>
+  </si>
+  <si>
+    <t>102 Foreign Special Relationships: Negative</t>
+  </si>
+  <si>
+    <t>302 Centralisation: Positive</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
@@ -443,7 +488,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -459,7 +504,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -475,7 +520,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -487,7 +532,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -504,9 +549,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -534,31 +579,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -586,23 +614,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -755,19 +766,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CU4"/>
+  <dimension ref="A1:CU7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="99" width="21.5546875" customWidth="1"/>
+    <col min="1" max="99" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1066,7 +1077,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>42809.683977175926</v>
       </c>
@@ -1365,7 +1376,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>42821.016064976851</v>
       </c>
@@ -1664,7 +1675,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>42822.923949166667</v>
       </c>
@@ -1963,7 +1974,904 @@
         <v>107</v>
       </c>
     </row>
+    <row r="5" spans="1:99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>42822.991386597219</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AG5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AH5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AI5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AK5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AL5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AM5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AN5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AO5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AQ5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AR5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AS5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AT5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AU5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AV5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AW5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AX5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AY5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AZ5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BA5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BB5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BC5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="BD5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BE5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BF5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="BG5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="BH5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="BI5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BJ5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="BK5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="BL5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="BM5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BN5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BO5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="BP5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="BQ5" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="BR5" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BS5" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="BT5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="BU5" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="BV5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="BW5" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="BX5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="BY5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="BZ5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CA5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="CB5" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="CC5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CD5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CE5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CF5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CG5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CH5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CI5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CJ5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CK5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="CL5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="CM5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CN5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="CO5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CP5" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="CQ5" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="CR5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CS5" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="CT5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="CU5" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>42823.004877025465</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AF6" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AG6" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AH6" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AI6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK6" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL6" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AM6" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AO6" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP6" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AQ6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AR6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AS6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AT6" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AU6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AV6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AW6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AX6" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AY6" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AZ6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="BA6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="BB6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="BC6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="BD6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="BE6" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="BF6" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="BG6" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="BH6" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="BI6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="BJ6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="BK6" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="BL6" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="BM6" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="BN6" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="BO6" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="BP6" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="BQ6" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="BR6" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="BS6" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="BT6" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="BU6" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="BV6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="BW6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="BX6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="BY6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="BZ6" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CA6" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CB6" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CC6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="CD6" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="CE6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CF6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="CG6" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="CH6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="CI6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CJ6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CK6" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="CL6" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="CM6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="CN6" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="CO6" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="CP6" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="CQ6" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="CR6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CS6" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="CT6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="CU6" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>42823.046213449074</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AG7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AH7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AJ7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AK7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AL7" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AM7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AN7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AO7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AQ7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AR7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AS7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AT7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AV7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AW7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AX7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AY7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AZ7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="BA7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="BB7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="BC7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="BD7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BE7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BF7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BG7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BH7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="BI7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BJ7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BK7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BL7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BM7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BN7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="BO7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BP7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="BQ7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BR7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="BS7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="BT7" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="BU7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="BV7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BW7" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="BX7" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="BY7" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="BZ7" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CA7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="CB7" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CC7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="CD7" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CE7" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CF7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="CG7" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="CH7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="CI7" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="CJ7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="CK7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="CL7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="CM7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="CN7" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="CO7" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="CP7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="CQ7" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="CR7" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="CS7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="CT7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="CU7" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>